<commit_message>
Enhance ScanWindow UI with dark mode support and improved layout; add filter functionality
</commit_message>
<xml_diff>
--- a/Sessions/2nd October session 2.xlsx
+++ b/Sessions/2nd October session 2.xlsx
@@ -517,16 +517,8 @@
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>[23:21:07]</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>[23:21:07] Denied Entry: No Exam &amp; Homework.</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>excel_import</t>
@@ -561,16 +553,8 @@
           <t>null 2</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>attend</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>[23:21:08]</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>

</xml_diff>